<commit_message>
scrn shot faliur issue
</commit_message>
<xml_diff>
--- a/src/main/java/testData/testdata_Excel.xlsx
+++ b/src/main/java/testData/testdata_Excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\eclipse-workspace\QA_Legend\src\main\java\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{745DE046-6DF1-4D50-9A89-DDAD7614FB23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A935450C-6BF6-4098-8BF0-D48EF70900A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -517,8 +517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9ACB6E6-EB46-472D-9DB5-EB77ADA869E4}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -647,7 +647,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06072F31-4CEF-44E0-86BA-B0B9A7FC7948}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>